<commit_message>
copy and add Worksheet
</commit_message>
<xml_diff>
--- a/public/uploads/hello.xlsx
+++ b/public/uploads/hello.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="First Sheet" sheetId="1" r:id="rId4"/>
-    <sheet name="Second Sheet" sheetId="2" r:id="rId5"/>
+    <sheet name="Copy Sheet" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
@@ -16,12 +16,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1">
   <si>
     <t>Hello World!</t>
-  </si>
-  <si>
-    <t>New Sheet</t>
   </si>
 </sst>
 </file>
@@ -401,7 +398,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SET DATA FROM ARRAY INTO CELLS
</commit_message>
<xml_diff>
--- a/public/uploads/hello.xlsx
+++ b/public/uploads/hello.xlsx
@@ -8,7 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="First Sheet" sheetId="1" r:id="rId4"/>
-    <sheet name="Copy Sheet" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
@@ -16,11 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1">
-  <si>
-    <t>Hello World!</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="0"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -354,7 +349,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -362,43 +357,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>0</v>
+    <row r="1" spans="1:2">
+      <c r="B1">
+        <v>100</v>
       </c>
     </row>
-  </sheetData>
-  <printOptions gridLines="false" gridLinesSet="true"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
-  <tableParts count="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>0</v>
+    <row r="2" spans="1:2">
+      <c r="B2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="B3">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Merge Unmerge Insert Col & Row
</commit_message>
<xml_diff>
--- a/public/uploads/hello.xlsx
+++ b/public/uploads/hello.xlsx
@@ -15,7 +15,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="0"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
+  <si>
+    <t>Hello, this is a very very long string.</t>
+  </si>
+  <si>
+    <t>World!</t>
+  </si>
+  <si>
+    <t>Bar</t>
+  </si>
+  <si>
+    <t>Foo</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -349,7 +362,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -358,27 +371,33 @@
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="B1">
-        <v>100</v>
+      <c r="B1" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="B2">
-        <v>53</v>
+      <c r="B2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="B3">
-        <v>86</v>
+      <c r="B3"/>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="B4" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="B4">
-        <f>SUM(B1:B3)</f>
-        <v>239</v>
+    <row r="5" spans="1:2">
+      <c r="B5" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:C2"/>
+  </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
visibility column and Row
</commit_message>
<xml_diff>
--- a/public/uploads/hello.xlsx
+++ b/public/uploads/hello.xlsx
@@ -369,6 +369,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="9.10" hidden="true" style="0"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" t="s">
@@ -383,7 +386,7 @@
     <row r="3" spans="1:2">
       <c r="B3"/>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" hidden="true">
       <c r="B4" t="s">
         <v>3</v>
       </c>

</xml_diff>